<commit_message>
Put watermark in PO, RFQ and AOQ and fix aoq_four and aoq_five
</commit_message>
<xml_diff>
--- a/AOQ.xlsx
+++ b/AOQ.xlsx
@@ -15,43 +15,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="83">
   <si>
     <t>ABSTRACT OF QUOTATION</t>
   </si>
   <si>
-    <t>Department: Admin</t>
-  </si>
-  <si>
-    <t>Date: August 5, 2019</t>
-  </si>
-  <si>
-    <t>Purpose: Lorem Ipsum Dolor</t>
-  </si>
-  <si>
-    <t>PR#: ADM19-1000</t>
-  </si>
-  <si>
-    <t>Enduse: enduse enduse enduse</t>
+    <t>Department: IT Department - BCD</t>
+  </si>
+  <si>
+    <t>Date: August 13, 2019</t>
+  </si>
+  <si>
+    <t>Purpose: TEST PURPOSE</t>
+  </si>
+  <si>
+    <t>PR#: IT Department - BCD19-1000</t>
+  </si>
+  <si>
+    <t>Enduse: TEST ENDUSE</t>
   </si>
   <si>
     <t xml:space="preserve">Date Needed: </t>
   </si>
   <si>
-    <t>Requested By: Lloyd Jamero/Jushkyle Jambongana</t>
-  </si>
-  <si>
-    <t>2GO Express
-(034) 704-1339</t>
-  </si>
-  <si>
-    <t>7RJ Brothers Sand &amp; Gravel &amp; Gen. Mdse.
-Ms. Tata
-(034)458-0190/213-2249</t>
-  </si>
-  <si>
-    <t>A.C. Parts Merchandising
-(034) 433-2512</t>
+    <t>Requested By: Stephine David Severino</t>
   </si>
   <si>
     <t>A-1 Gas Corporation
@@ -59,6 +46,20 @@
 434-0708; 433-3637; 433-3638; 432-2079</t>
   </si>
   <si>
+    <t>AA Electrical Supply
+Rene 
+435-3811; 432-3712; 708-1212</t>
+  </si>
+  <si>
+    <t>Ablao Enterprises
+461-0376</t>
+  </si>
+  <si>
+    <t>Abomar Equipment Sales Corporation
+Danilo Palomar
+433-1687; 432-3673</t>
+  </si>
+  <si>
     <t>#</t>
   </si>
   <si>
@@ -83,93 +84,174 @@
     <t>COMMENTS</t>
   </si>
   <si>
-    <t>Laptop Charger</t>
-  </si>
-  <si>
-    <t>unit/s</t>
-  </si>
-  <si>
-    <t>2GO Express, Laptop Charger</t>
-  </si>
-  <si>
-    <t>7RJ Brothers, Laptop Charger</t>
-  </si>
-  <si>
-    <t>A.C. Parts Merchandising, Laptop Charger</t>
-  </si>
-  <si>
-    <t>A-1 Gas, Laptop Charger</t>
-  </si>
-  <si>
-    <t>2GO Express1, Laptop Charger</t>
-  </si>
-  <si>
-    <t>7RJ Brothers1, Laptop Charger</t>
-  </si>
-  <si>
-    <t>A.C. Parts Merchandising1, Laptop Charger</t>
-  </si>
-  <si>
-    <t>USB</t>
-  </si>
-  <si>
-    <t>2GO Express2, USB</t>
-  </si>
-  <si>
-    <t>7RJ Brothers3, USB</t>
-  </si>
-  <si>
-    <t>A.C. Parts Merchandising2, USB</t>
-  </si>
-  <si>
-    <t>A-1 Gas1, USB</t>
-  </si>
-  <si>
-    <t>2GO Express3, USB</t>
-  </si>
-  <si>
-    <t>7RJ Brothers4, USB</t>
-  </si>
-  <si>
-    <t>Wifi Adapter</t>
-  </si>
-  <si>
-    <t>2GO Express4, Wifi Adapter</t>
-  </si>
-  <si>
-    <t>7RJ Brothers6, Wifi Adapter</t>
-  </si>
-  <si>
-    <t>A.C. Parts Merchandising3, Wifi Adapter</t>
-  </si>
-  <si>
-    <t>A-1 Gas2, Wifi Adapter</t>
-  </si>
-  <si>
-    <t>2GO Express5, Wifi Adapter</t>
-  </si>
-  <si>
-    <t>7RJ Brothers7, Wifi Adapter</t>
-  </si>
-  <si>
-    <t>7RJ Brothers8, Wifi Adapter</t>
+    <t>Test Ballpen</t>
+  </si>
+  <si>
+    <t>pc/s</t>
+  </si>
+  <si>
+    <t>A-1 Gas, Test Ballpen</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>AA Electrical, Test Ballpen</t>
+  </si>
+  <si>
+    <t>Ablao, Test Ballpen</t>
+  </si>
+  <si>
+    <t>Abomar, Test Ballpen</t>
+  </si>
+  <si>
+    <t>A-1 Gas1, Test Ballpen</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>Ablao1, Test Ballpen</t>
+  </si>
+  <si>
+    <t>Ablao2, Test Ballpen</t>
+  </si>
+  <si>
+    <t>Test Monitor</t>
+  </si>
+  <si>
+    <t>A-1 Gas2, Test Monitor</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>AA Electrical1, Test Monitor</t>
+  </si>
+  <si>
+    <t>Ablao3, Test Monitor</t>
+  </si>
+  <si>
+    <t>Abomar1, Test Monitor</t>
+  </si>
+  <si>
+    <t>AA Electrica2l, Test Monitor</t>
+  </si>
+  <si>
+    <t>Abomar2, Test Monitor</t>
+  </si>
+  <si>
+    <t>AA Electrical3, Test Monitor</t>
+  </si>
+  <si>
+    <t>Test Paper</t>
+  </si>
+  <si>
+    <t>A-1 Gas3, Test Paper</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>AA Electrical4, Test Paper</t>
+  </si>
+  <si>
+    <t>Ablao4, Test Paper</t>
+  </si>
+  <si>
+    <t>Abomar3, Test Paper</t>
+  </si>
+  <si>
+    <t>A-1 Gas4, Test Paper</t>
+  </si>
+  <si>
+    <t>test4</t>
+  </si>
+  <si>
+    <t>Ablao5, Test Paper</t>
+  </si>
+  <si>
+    <t>A-1 Gas5, Test Paper</t>
+  </si>
+  <si>
+    <t>test5</t>
   </si>
   <si>
     <t>a. Price Validity</t>
   </si>
   <si>
+    <t>test price</t>
+  </si>
+  <si>
+    <t>test price1</t>
+  </si>
+  <si>
+    <t>test price2</t>
+  </si>
+  <si>
+    <t>test price3</t>
+  </si>
+  <si>
     <t>b. Payment Terms</t>
   </si>
   <si>
+    <t>Terms</t>
+  </si>
+  <si>
+    <t>Terms1</t>
+  </si>
+  <si>
+    <t>Terms2</t>
+  </si>
+  <si>
+    <t>Terms3</t>
+  </si>
+  <si>
     <t>c. Date of Delivery</t>
   </si>
   <si>
-    <t>August 5, 2019</t>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Time1</t>
+  </si>
+  <si>
+    <t>Time2</t>
+  </si>
+  <si>
+    <t>Time3</t>
   </si>
   <si>
     <t>d. Items Warranty</t>
   </si>
   <si>
+    <t>Warranty</t>
+  </si>
+  <si>
+    <t>Warranty1</t>
+  </si>
+  <si>
+    <t>Warranty2</t>
+  </si>
+  <si>
+    <t>Warranty3</t>
+  </si>
+  <si>
+    <t>e. In-land Freight</t>
+  </si>
+  <si>
+    <t>Freight</t>
+  </si>
+  <si>
+    <t>Freight1</t>
+  </si>
+  <si>
+    <t>Freight2</t>
+  </si>
+  <si>
+    <t>Freight3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Prepared by: </t>
   </si>
   <si>
@@ -185,13 +267,10 @@
     <t>Jonah Benares</t>
   </si>
   <si>
-    <t>Lloyd Jamero/Jushkyle Jambongana</t>
-  </si>
-  <si>
-    <t>Caesariane Jo</t>
-  </si>
-  <si>
-    <t>Concordio Matuod</t>
+    <t>Stephine David Severino</t>
+  </si>
+  <si>
+    <t>Celina Marie Grabillo</t>
   </si>
 </sst>
 </file>
@@ -630,7 +709,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:W27"/>
+  <dimension ref="A1:W26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A8" sqref="A8"/>
@@ -639,22 +718,22 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="2.285156" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="17.567139" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="55.272217" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="15.281982" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="44.703369" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="6.998291" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="38.847656" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="24.708252" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="35.2771" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="8.140869" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="19.995117" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="28.135986" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="37.705078" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="34.134521" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="6.998291" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="25.85083" bestFit="true" customWidth="true" style="0"/>
     <col min="12" max="12" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="49.416504" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="8.140869" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="24.708252" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="6.998291" bestFit="true" customWidth="true" style="0"/>
     <col min="15" max="15" width="8.140869" bestFit="true" customWidth="true" style="0"/>
     <col min="16" max="16" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="28.135986" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="8.140869" bestFit="true" customWidth="true" style="0"/>
-    <col min="19" max="19" width="10.568848" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="25.85083" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="6.998291" bestFit="true" customWidth="true" style="0"/>
+    <col min="19" max="19" width="8.140869" bestFit="true" customWidth="true" style="0"/>
     <col min="20" max="20" width="10.568848" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
@@ -791,7 +870,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>21</v>
@@ -800,40 +879,42 @@
         <v>22</v>
       </c>
       <c r="F9" s="5">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G9" s="6">
+        <v>10</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="7">
-        <v>31</v>
+      <c r="J9" s="5">
+        <v>10</v>
       </c>
       <c r="K9" s="7">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N9" s="7">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="O9" s="7">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="P9" s="2"/>
       <c r="Q9" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R9" s="7">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S9" s="7">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="T9" s="2"/>
       <c r="V9" s="9"/>
@@ -845,33 +926,29 @@
       <c r="C10" s="4"/>
       <c r="D10" s="2"/>
       <c r="E10" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F10" s="7">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G10" s="7">
-        <v>26</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J10" s="5">
-        <v>12</v>
-      </c>
-      <c r="K10" s="7">
-        <v>24</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
       <c r="L10" s="2"/>
       <c r="M10" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N10" s="7">
-        <v>334</v>
+        <v>13</v>
       </c>
       <c r="O10" s="7">
-        <v>668</v>
+        <v>13</v>
       </c>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
@@ -882,148 +959,124 @@
       <c r="W10" s="9"/>
     </row>
     <row r="11" spans="1:23">
-      <c r="A11" s="2">
-        <v>2</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="4">
-        <v>5</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="7">
-        <v>14</v>
-      </c>
-      <c r="G11" s="6">
-        <v>70</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J11" s="7">
-        <v>123</v>
-      </c>
-      <c r="K11" s="7">
-        <v>615</v>
-      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
       <c r="L11" s="2"/>
       <c r="M11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="N11" s="5">
-        <v>12</v>
+        <v>30</v>
+      </c>
+      <c r="N11" s="7">
+        <v>14</v>
       </c>
       <c r="O11" s="7">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="P11" s="2"/>
-      <c r="Q11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="R11" s="7">
-        <v>424</v>
-      </c>
-      <c r="S11" s="7">
-        <v>2120</v>
-      </c>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
       <c r="T11" s="2"/>
       <c r="V11" s="9"/>
       <c r="W11" s="9"/>
     </row>
     <row r="12" spans="1:23">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="2"/>
+      <c r="A12" s="2">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="4">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="E12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="5">
+        <v>12</v>
+      </c>
+      <c r="G12" s="6">
+        <v>48</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="7">
-        <v>15</v>
-      </c>
-      <c r="G12" s="7">
-        <v>75</v>
-      </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="3" t="s">
+      <c r="J12" s="7">
+        <v>13</v>
+      </c>
+      <c r="K12" s="7">
+        <v>52</v>
+      </c>
+      <c r="L12" s="2"/>
+      <c r="M12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J12" s="7">
-        <v>43</v>
-      </c>
-      <c r="K12" s="7">
-        <v>215</v>
-      </c>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
+      <c r="N12" s="7">
+        <v>14</v>
+      </c>
+      <c r="O12" s="7">
+        <v>56</v>
+      </c>
       <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
+      <c r="Q12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R12" s="5">
+        <v>12</v>
+      </c>
+      <c r="S12" s="7">
+        <v>48</v>
+      </c>
       <c r="T12" s="2"/>
       <c r="V12" s="9"/>
       <c r="W12" s="9"/>
     </row>
     <row r="13" spans="1:23">
-      <c r="A13" s="2">
-        <v>3</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="4">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="7">
-        <v>16</v>
-      </c>
-      <c r="G13" s="6">
-        <v>16</v>
-      </c>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
       <c r="H13" s="2"/>
       <c r="I13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J13" s="5">
-        <v>12</v>
+        <v>37</v>
+      </c>
+      <c r="J13" s="7">
+        <v>14</v>
       </c>
       <c r="K13" s="7">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="L13" s="2"/>
-      <c r="M13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="N13" s="7">
-        <v>13</v>
-      </c>
-      <c r="O13" s="7">
-        <v>13</v>
-      </c>
+      <c r="M13" s="2"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="R13" s="7">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="S13" s="7">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="T13" s="2"/>
       <c r="V13" s="9"/>
@@ -1034,24 +1087,18 @@
       <c r="B14" s="2"/>
       <c r="C14" s="4"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="7">
-        <v>17</v>
-      </c>
-      <c r="G14" s="7">
-        <v>17</v>
-      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
       <c r="H14" s="2"/>
       <c r="I14" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J14" s="7">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="K14" s="7">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
@@ -1065,165 +1112,288 @@
       <c r="V14" s="9"/>
       <c r="W14" s="9"/>
     </row>
-    <row r="15" spans="1:23">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="3" t="s">
+    <row r="16" spans="1:23">
+      <c r="A16" s="2">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="4">
+        <v>15</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="7">
+        <v>13</v>
+      </c>
+      <c r="G16" s="7">
+        <v>195</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="J15" s="7">
-        <v>112</v>
-      </c>
-      <c r="K15" s="7">
-        <v>112</v>
-      </c>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="2"/>
-      <c r="V15" s="9"/>
-      <c r="W15" s="9"/>
+      <c r="J16" s="7">
+        <v>14</v>
+      </c>
+      <c r="K16" s="7">
+        <v>210</v>
+      </c>
+      <c r="L16" s="2"/>
+      <c r="M16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="N16" s="7">
+        <v>15</v>
+      </c>
+      <c r="O16" s="7">
+        <v>225</v>
+      </c>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="R16" s="7">
+        <v>13</v>
+      </c>
+      <c r="S16" s="7">
+        <v>195</v>
+      </c>
+      <c r="T16" s="2"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
     </row>
     <row r="17" spans="1:23">
-      <c r="C17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="15">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="7">
+        <v>13.5</v>
+      </c>
+      <c r="G17" s="7">
+        <v>202.5</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="N17" s="7">
+        <v>16</v>
+      </c>
+      <c r="O17" s="7">
+        <v>240</v>
+      </c>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="2"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+    </row>
+    <row r="18" spans="1:23">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="5">
         <v>12</v>
       </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17"/>
-      <c r="I17" s="15">
-        <v>312</v>
-      </c>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
-      <c r="M17" s="15">
-        <v>123</v>
-      </c>
-      <c r="N17" s="16"/>
-      <c r="O17" s="16"/>
-      <c r="Q17" s="15">
-        <v>123</v>
-      </c>
-      <c r="R17" s="16"/>
-      <c r="S17" s="16"/>
-    </row>
-    <row r="19" spans="1:23">
-      <c r="C19" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" s="15">
-        <v>34</v>
-      </c>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="I19" s="15">
+      <c r="G18" s="6">
+        <v>180</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="2"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9"/>
+    </row>
+    <row r="20" spans="1:23">
+      <c r="C20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20"/>
+      <c r="I20" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="M20" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-      <c r="L19"/>
-      <c r="M19" s="15">
-        <v>12</v>
-      </c>
-      <c r="N19" s="16"/>
-      <c r="O19" s="16"/>
-      <c r="Q19" s="15">
-        <v>32</v>
-      </c>
-      <c r="R19" s="16"/>
-      <c r="S19" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="Q20" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="R20" s="16"/>
+      <c r="S20" s="16"/>
     </row>
     <row r="21" spans="1:23">
       <c r="C21" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
       <c r="I21" s="15" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="J21" s="16"/>
       <c r="K21" s="16"/>
+      <c r="L21"/>
       <c r="M21" s="15" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="N21" s="16"/>
       <c r="O21" s="16"/>
-      <c r="P21"/>
       <c r="Q21" s="15" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="R21" s="16"/>
       <c r="S21" s="16"/>
     </row>
+    <row r="22" spans="1:23">
+      <c r="C22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="I22" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="M22" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22"/>
+      <c r="Q22" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="R22" s="16"/>
+      <c r="S22" s="16"/>
+    </row>
     <row r="23" spans="1:23">
       <c r="C23" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="15">
-        <v>1</v>
+        <v>66</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>67</v>
       </c>
       <c r="F23" s="16"/>
       <c r="G23" s="16"/>
-      <c r="I23" s="15">
-        <v>2</v>
+      <c r="I23" s="15" t="s">
+        <v>68</v>
       </c>
       <c r="J23" s="16"/>
       <c r="K23" s="16"/>
-      <c r="M23" s="15">
-        <v>3</v>
+      <c r="M23" s="15" t="s">
+        <v>69</v>
       </c>
       <c r="N23" s="16"/>
       <c r="O23" s="16"/>
-      <c r="Q23" s="15">
-        <v>4</v>
+      <c r="Q23" s="15" t="s">
+        <v>70</v>
       </c>
       <c r="R23" s="16"/>
       <c r="S23" s="16"/>
     </row>
+    <row r="24" spans="1:23">
+      <c r="C24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="I24" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="M24" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="Q24" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="R24" s="16"/>
+      <c r="S24" s="16"/>
+    </row>
     <row r="25" spans="1:23">
       <c r="E25" s="8" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23">
-      <c r="E27" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="G27" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="I27" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="K27" s="17" t="s">
-        <v>56</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23">
+      <c r="E26" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="I26" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="K26" s="17" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1234,9 +1404,9 @@
     <mergeCell ref="I7:L7"/>
     <mergeCell ref="M7:P7"/>
     <mergeCell ref="Q7:T7"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="I19:L19"/>
-    <mergeCell ref="M21:P21"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="I21:L21"/>
+    <mergeCell ref="M22:P22"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
po draft, pr summary report qty per dr and revise qty, po offer only, qty in rfq, due date in pr group
</commit_message>
<xml_diff>
--- a/AOQ.xlsx
+++ b/AOQ.xlsx
@@ -15,43 +15,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
   <si>
     <t>ABSTRACT OF QUOTATION</t>
   </si>
   <si>
-    <t>Department: Operations</t>
-  </si>
-  <si>
-    <t>Date: September 25, 2019</t>
-  </si>
-  <si>
-    <t>Purpose: Consumbles for Rewinding of Rotor Pole #2 (Supersede).</t>
-  </si>
-  <si>
-    <t>PR#: EIC19-1003</t>
-  </si>
-  <si>
-    <t>Enduse: DG3 Main Field/Rotor.</t>
+    <t>Department: Accounting</t>
+  </si>
+  <si>
+    <t>Date: October 2, 2019</t>
+  </si>
+  <si>
+    <t>Purpose: Sample Purpose</t>
+  </si>
+  <si>
+    <t>PR#: acc19-1000</t>
+  </si>
+  <si>
+    <t>Enduse: Sample Enduse</t>
   </si>
   <si>
     <t xml:space="preserve">Date Needed: </t>
   </si>
   <si>
-    <t>Requested By: Julius Pangilinan / Kennah Sasamoto</t>
-  </si>
-  <si>
-    <t>Ace Hardware Philippines, Inc. - Bacolod Branch
-(034) 468 0135</t>
-  </si>
-  <si>
-    <t>A-one Industrial Sales
-Ms. Miles
-435-7383; 432-0652; 476-1127</t>
-  </si>
-  <si>
-    <t>Visayan Construction Supply
-434-7277 / 434-7278</t>
+    <t>Requested By: Henne Tanan</t>
+  </si>
+  <si>
+    <t>Bacolod China Mart
+Ms. Donna/Ms, Angela
+434-7293/434-7670</t>
+  </si>
+  <si>
+    <t>Bacolod Office Solutions Unlimited, Inc.
+433-9636</t>
+  </si>
+  <si>
+    <t>Bacolod HKL Enterprises
+(034) 458 9588</t>
   </si>
   <si>
     <t>#</t>
@@ -78,37 +78,28 @@
     <t>COMMENTS</t>
   </si>
   <si>
-    <t>Plier; Electrical</t>
-  </si>
-  <si>
-    <t>pc.</t>
-  </si>
-  <si>
-    <t>Ace Hardware</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A-one Industrial </t>
-  </si>
-  <si>
-    <t>Visayan Construction</t>
-  </si>
-  <si>
-    <t>Ace Hardware1</t>
-  </si>
-  <si>
-    <t>A-one Industrial1</t>
-  </si>
-  <si>
-    <t>Visayan Construction1</t>
-  </si>
-  <si>
-    <t>Ace Hardware2</t>
-  </si>
-  <si>
-    <t>A-one Industrial2</t>
-  </si>
-  <si>
-    <t>Visayan Construction2</t>
+    <t>Ballpen</t>
+  </si>
+  <si>
+    <t>bcm ballpen offer</t>
+  </si>
+  <si>
+    <t>bosu ballpen offer</t>
+  </si>
+  <si>
+    <t>hkl ballpen offer</t>
+  </si>
+  <si>
+    <t>Envelope</t>
+  </si>
+  <si>
+    <t>bcm envelope offer</t>
+  </si>
+  <si>
+    <t>bosu envelope offer</t>
+  </si>
+  <si>
+    <t>hkl envelope offer</t>
   </si>
   <si>
     <t>a. Price Validity</t>
@@ -141,13 +132,13 @@
     <t>Jonah Benares</t>
   </si>
   <si>
-    <t>Julius Pangilinan / Kennah Sasamoto</t>
-  </si>
-  <si>
-    <t>stephine david severino, jason flor, hennelen tana</t>
-  </si>
-  <si>
-    <t>charmaine plaza, kervic salas, maylen cabaylo</t>
+    <t>Henne Tanan</t>
+  </si>
+  <si>
+    <t>jonah benares</t>
+  </si>
+  <si>
+    <t>mila arana/david tan</t>
   </si>
 </sst>
 </file>
@@ -184,7 +175,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,12 +188,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFf4e542"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -232,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -249,9 +234,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="4" fillId="2" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="4" fillId="3" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
@@ -583,7 +565,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:W22"/>
+  <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A8" sqref="A8"/>
@@ -592,16 +574,16 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="2.285156" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="21.137695" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="75.410156" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="13.996582" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="30.563965" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="6.998291" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="42.418213" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="29.421387" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="60.128174" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="26.993408" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="25.85083" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="23.422852" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="6.998291" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="54.129639" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="24.708252" bestFit="true" customWidth="true" style="0"/>
     <col min="12" max="12" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="25.85083" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="22.280273" bestFit="true" customWidth="true" style="0"/>
     <col min="14" max="14" width="6.998291" bestFit="true" customWidth="true" style="0"/>
     <col min="15" max="15" width="8.140869" bestFit="true" customWidth="true" style="0"/>
     <col min="16" max="16" width="10.568848" bestFit="true" customWidth="true" style="0"/>
@@ -643,72 +625,72 @@
       </c>
     </row>
     <row r="7" spans="1:23" customHeight="1" ht="50">
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="11" t="s">
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="11" t="s">
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="11"/>
     </row>
     <row r="8" spans="1:23">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="K8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="L8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="M8" s="10" t="s">
+      <c r="M8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="10" t="s">
+      <c r="N8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="O8" s="10" t="s">
+      <c r="O8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="P8" s="10" t="s">
+      <c r="P8" s="9" t="s">
         <v>18</v>
       </c>
     </row>
@@ -720,231 +702,195 @@
         <v>19</v>
       </c>
       <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="F9" s="5">
         <v>10</v>
       </c>
       <c r="G9" s="6">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" s="7">
-        <v>40</v>
-      </c>
-      <c r="K9" s="7">
-        <v>40</v>
+        <v>21</v>
+      </c>
+      <c r="J9" s="6">
+        <v>14</v>
+      </c>
+      <c r="K9" s="6">
+        <v>70</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" s="6">
+        <v>15</v>
+      </c>
+      <c r="O9" s="6">
+        <v>75</v>
+      </c>
+      <c r="P9" s="2"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+    </row>
+    <row r="12" spans="1:23">
+      <c r="A12" s="2">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="N9" s="7">
-        <v>70</v>
-      </c>
-      <c r="O9" s="7">
-        <v>70</v>
-      </c>
-      <c r="P9" s="2"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
-      <c r="V9" s="9"/>
-      <c r="W9" s="9"/>
-    </row>
-    <row r="10" spans="1:23">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="3" t="s">
+      <c r="C12" s="4">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="7">
-        <v>20</v>
-      </c>
-      <c r="G10" s="7">
-        <v>20</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="3" t="s">
+      <c r="F12" s="6">
+        <v>13.5</v>
+      </c>
+      <c r="G12" s="6">
+        <v>54</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J10" s="7">
-        <v>50</v>
-      </c>
-      <c r="K10" s="7">
-        <v>50</v>
-      </c>
-      <c r="L10" s="2"/>
-      <c r="M10" s="3" t="s">
+      <c r="J12" s="5">
+        <v>12</v>
+      </c>
+      <c r="K12" s="6">
+        <v>48</v>
+      </c>
+      <c r="L12" s="2"/>
+      <c r="M12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="N10" s="7">
-        <v>80</v>
-      </c>
-      <c r="O10" s="7">
-        <v>80</v>
-      </c>
-      <c r="P10" s="2"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="9"/>
-    </row>
-    <row r="11" spans="1:23">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="7">
-        <v>30</v>
-      </c>
-      <c r="G11" s="7">
-        <v>30</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" s="7">
-        <v>60</v>
-      </c>
-      <c r="K11" s="7">
-        <v>60</v>
-      </c>
-      <c r="L11" s="2"/>
-      <c r="M11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N11" s="7">
-        <v>90</v>
-      </c>
-      <c r="O11" s="7">
-        <v>90</v>
-      </c>
-      <c r="P11" s="2"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
-      <c r="V11" s="9"/>
-      <c r="W11" s="9"/>
-    </row>
-    <row r="15" spans="1:23">
-      <c r="C15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
+      <c r="N12" s="6">
+        <v>16.5</v>
+      </c>
+      <c r="O12" s="6">
+        <v>66</v>
+      </c>
+      <c r="P12" s="2"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
     </row>
     <row r="16" spans="1:23">
       <c r="C16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
+        <v>27</v>
+      </c>
+      <c r="E16" s="13"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
     </row>
     <row r="17" spans="1:23">
       <c r="C17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17"/>
+        <v>28</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
     </row>
     <row r="18" spans="1:23">
       <c r="C18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="14"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
+        <v>29</v>
+      </c>
+      <c r="E18" s="13"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18"/>
     </row>
     <row r="19" spans="1:23">
       <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+    </row>
+    <row r="20" spans="1:23">
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+    </row>
+    <row r="21" spans="1:23">
+      <c r="E21" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I21" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
-    </row>
-    <row r="20" spans="1:23">
-      <c r="E20" s="8" t="s">
+      <c r="K21" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G20" s="8" t="s">
+    </row>
+    <row r="22" spans="1:23">
+      <c r="E22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="K22" s="15"/>
+    </row>
+    <row r="23" spans="1:23">
+      <c r="E23" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="G23" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="K20" s="8" t="s">
+      <c r="I23" s="7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="21" spans="1:23">
-      <c r="E21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="K21" s="16"/>
-    </row>
-    <row r="22" spans="1:23">
-      <c r="E22" s="8" t="s">
+      <c r="K23" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="K22" s="8" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -954,9 +900,9 @@
     <mergeCell ref="E7:H7"/>
     <mergeCell ref="I7:L7"/>
     <mergeCell ref="M7:P7"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="I16:L16"/>
-    <mergeCell ref="M17:P17"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="I17:L17"/>
+    <mergeCell ref="M18:P18"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix error in aoq and issuance
</commit_message>
<xml_diff>
--- a/AOQ.xlsx
+++ b/AOQ.xlsx
@@ -15,12 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
   <si>
     <t>ABSTRACT OF QUOTATION</t>
   </si>
   <si>
-    <t>JO No.: IT</t>
+    <t>JO No.: JOR 2021-5-CNPR</t>
   </si>
   <si>
     <t>Project Title: Testing only</t>
@@ -80,13 +80,6 @@
   </si>
   <si>
     <t>pc/s</t>
-  </si>
-  <si>
-    <t>Supply of labor, testing tools and technical expertise for the Configuration of EasyGen Relay on SSR125 AVR at DG 4 &amp; DG 5.
-Scope of works include but not limited to the following:
-1. Wiring of Signal from EasyGen to AVR
-2. Configuration of EasyGen relay for excitation of On-Load and Off-Load step response.
-3. Simulation and Functional Test.</t>
   </si>
   <si>
     <t>PHP</t>
@@ -226,7 +219,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,6 +232,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFf4e542"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -268,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -282,6 +281,9 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="4" fillId="2" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="4" fillId="3" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
@@ -653,131 +655,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="E1" s="13"/>
+      <c r="E1" s="14"/>
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="J1" s="13"/>
-      <c r="O1" s="13"/>
+      <c r="J1" s="14"/>
+      <c r="O1" s="14"/>
     </row>
     <row r="2" spans="1:19">
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="O2" s="13"/>
+      <c r="E2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="O2" s="14"/>
     </row>
     <row r="3" spans="1:19">
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="O3" s="13"/>
+      <c r="E3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="O3" s="14"/>
     </row>
     <row r="4" spans="1:19">
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="O4" s="13"/>
+      <c r="E4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="O4" s="14"/>
     </row>
     <row r="5" spans="1:19">
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="O5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="O5" s="14"/>
     </row>
     <row r="6" spans="1:19">
-      <c r="E6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="O6" s="13"/>
+      <c r="E6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="O6" s="14"/>
     </row>
     <row r="7" spans="1:19" customHeight="1" ht="50">
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="8" t="s">
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="8" t="s">
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="9"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="10"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="K8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="L8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="7" t="s">
+      <c r="M8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="7" t="s">
+      <c r="N8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="O8" s="8" t="s">
+      <c r="O8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P8" s="7" t="s">
+      <c r="P8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="Q8" s="7" t="s">
+      <c r="Q8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="R8" s="7" t="s">
+      <c r="R8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="S8" s="7" t="s">
+      <c r="S8" s="8" t="s">
         <v>16</v>
       </c>
     </row>
@@ -785,20 +787,20 @@
       <c r="A9" s="2">
         <v>1</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="11">
         <v>1</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="16">
+        <v>100</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="G9" s="4">
         <v>100</v>
@@ -807,141 +809,141 @@
         <v>100</v>
       </c>
       <c r="I9" s="2"/>
-      <c r="J9" s="15" t="s">
-        <v>21</v>
+      <c r="J9" s="16" t="s">
+        <v>20</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L9" s="5">
+        <v>19</v>
+      </c>
+      <c r="L9" s="6">
         <v>300</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="6">
         <v>300</v>
       </c>
       <c r="N9" s="2"/>
-      <c r="O9" s="15">
+      <c r="O9" s="16">
         <v>600</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q9" s="5">
+        <v>19</v>
+      </c>
+      <c r="Q9" s="6">
         <v>800</v>
       </c>
-      <c r="R9" s="5">
+      <c r="R9" s="6">
         <v>800</v>
       </c>
       <c r="S9" s="2"/>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="2"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="15">
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="16">
         <v>200</v>
       </c>
       <c r="F10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="6">
+        <v>200</v>
+      </c>
+      <c r="H10" s="6">
+        <v>200</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="5">
-        <v>200</v>
-      </c>
-      <c r="H10" s="5">
-        <v>200</v>
-      </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="15" t="s">
-        <v>23</v>
-      </c>
       <c r="K10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L10" s="5">
+        <v>19</v>
+      </c>
+      <c r="L10" s="6">
         <v>400</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="6">
         <v>400</v>
       </c>
       <c r="N10" s="2"/>
-      <c r="O10" s="9"/>
+      <c r="O10" s="10"/>
       <c r="P10" s="3"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
       <c r="S10" s="2"/>
     </row>
     <row r="11" spans="1:19">
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="O11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="O11" s="14"/>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="2">
         <v>2</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="11">
+        <v>2</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="16">
+        <v>300</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="10">
-        <v>2</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="15">
+      <c r="G12" s="6">
+        <v>150</v>
+      </c>
+      <c r="H12" s="6">
         <v>300</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="I12" s="2"/>
+      <c r="J12" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="5">
-        <v>150</v>
-      </c>
-      <c r="H12" s="5">
-        <v>300</v>
-      </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="15" t="s">
-        <v>26</v>
-      </c>
       <c r="K12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L12" s="5">
+        <v>19</v>
+      </c>
+      <c r="L12" s="6">
         <v>500</v>
       </c>
-      <c r="M12" s="5">
+      <c r="M12" s="6">
         <v>1000</v>
       </c>
       <c r="N12" s="2"/>
-      <c r="O12" s="15">
+      <c r="O12" s="16">
         <v>700</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q12" s="5">
+        <v>19</v>
+      </c>
+      <c r="Q12" s="6">
         <v>900</v>
       </c>
-      <c r="R12" s="5">
+      <c r="R12" s="6">
         <v>1800</v>
       </c>
       <c r="S12" s="2"/>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="2"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="15">
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="16">
         <v>400</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G13" s="4">
         <v>56</v>
@@ -950,250 +952,250 @@
         <v>112</v>
       </c>
       <c r="I13" s="2"/>
-      <c r="J13" s="15" t="s">
-        <v>28</v>
+      <c r="J13" s="16" t="s">
+        <v>27</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L13" s="5">
+        <v>19</v>
+      </c>
+      <c r="L13" s="6">
         <v>450</v>
       </c>
-      <c r="M13" s="5">
+      <c r="M13" s="6">
         <v>900</v>
       </c>
       <c r="N13" s="2"/>
-      <c r="O13" s="9"/>
+      <c r="O13" s="10"/>
       <c r="P13" s="3"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
       <c r="S13" s="2"/>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="2"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="15">
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="16">
         <v>500</v>
       </c>
       <c r="F14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="6">
+        <v>155</v>
+      </c>
+      <c r="H14" s="6">
+        <v>310</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="2"/>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="O15" s="14"/>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="B16" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="J16" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="5">
-        <v>155</v>
-      </c>
-      <c r="H14" s="5">
-        <v>310</v>
-      </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="2"/>
-    </row>
-    <row r="15" spans="1:19">
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="O15" s="13"/>
-    </row>
-    <row r="16" spans="1:19">
-      <c r="B16" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="16" t="s">
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="O16" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="J16" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="O16" s="16" t="s">
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+    </row>
+    <row r="17" spans="1:19">
+      <c r="B17" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="11"/>
-    </row>
-    <row r="17" spans="1:19">
-      <c r="B17" s="13" t="s">
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="16" t="s">
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="J17" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="O17" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="J17" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="O17" s="16" t="s">
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+    </row>
+    <row r="18" spans="1:19">
+      <c r="B18" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
-    </row>
-    <row r="18" spans="1:19">
-      <c r="B18" s="13" t="s">
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="16" t="s">
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="J18" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="O18" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="J18" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="O18" s="16" t="s">
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+    </row>
+    <row r="19" spans="1:19">
+      <c r="B19" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11"/>
-      <c r="R18" s="11"/>
-    </row>
-    <row r="19" spans="1:19">
-      <c r="B19" s="13" t="s">
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="16" t="s">
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="J19" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="O19" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="J19" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="O19" s="16" t="s">
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="B20" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="11"/>
-    </row>
-    <row r="20" spans="1:19">
-      <c r="B20" s="13" t="s">
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="16" t="s">
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="J20" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="J20" s="16" t="s">
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="O20" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="O20" s="16" t="s">
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
+    </row>
+    <row r="21" spans="1:19">
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="O21" s="14"/>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="B22" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="11"/>
-    </row>
-    <row r="21" spans="1:19">
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="O21" s="13"/>
-    </row>
-    <row r="22" spans="1:19">
-      <c r="B22" s="13" t="s">
+      <c r="C22" s="14"/>
+      <c r="D22" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13" t="s">
+      <c r="E22" s="18"/>
+      <c r="G22" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="17"/>
-      <c r="G22" s="6" t="s">
+      <c r="H22"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="H22"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="6" t="s">
-        <v>48</v>
       </c>
       <c r="L22"/>
       <c r="M22"/>
-      <c r="O22" s="13" t="s">
+      <c r="O22" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
+      <c r="B23" s="15"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="19"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="O23" s="15"/>
+    </row>
+    <row r="24" spans="1:19">
+      <c r="B24" s="14" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="1:19">
-      <c r="B23" s="14"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="18"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="O23" s="14"/>
-    </row>
-    <row r="24" spans="1:19">
-      <c r="B24" s="13" t="s">
+      <c r="C24" s="14"/>
+      <c r="D24" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="18"/>
+      <c r="G24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" s="17"/>
-      <c r="G24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="6" t="s">
+      <c r="O24" s="14" t="s">
         <v>51</v>
-      </c>
-      <c r="O24" s="13" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix concerns in Need to fix sheet
</commit_message>
<xml_diff>
--- a/AOQ.xlsx
+++ b/AOQ.xlsx
@@ -15,34 +15,35 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
   <si>
     <t>ABSTRACT OF QUOTATION</t>
   </si>
   <si>
-    <t>JO No.: IT</t>
-  </si>
-  <si>
-    <t>Project Title: Testing only</t>
-  </si>
-  <si>
-    <t>Requested By: Stephine David Severino</t>
-  </si>
-  <si>
-    <t>Department: IT</t>
-  </si>
-  <si>
-    <t>A.M. Builders' Depot
-(034)709-0055</t>
-  </si>
-  <si>
-    <t>AA Electrical Supply
-Sir Rene 
-435-3811; 432-3712; 708-1212</t>
-  </si>
-  <si>
-    <t>Ablao Enterprises
-461-0376</t>
+    <t>JO No.: JOR 2021-1-CNPR</t>
+  </si>
+  <si>
+    <t>Project Title: SAMPLE PURPOSE BY HR ADMIN</t>
+  </si>
+  <si>
+    <t>Requested By: SAMPLE REQUEST BY HR ADMIN</t>
+  </si>
+  <si>
+    <t>Department: ITB</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tough Performance AutoWorkz
+(034) 432 0544 </t>
+  </si>
+  <si>
+    <t>2GO Express, Inc.
+Ms Apple/Ms Liza
+(034) 435-4965 / 704-2039 / 704-2396</t>
+  </si>
+  <si>
+    <t>7RJ Brothers Sand &amp; Gravel &amp; Gen. Mdse.
+Ms. Tata
+(034)458-0190/213-2249</t>
   </si>
   <si>
     <t>#</t>
@@ -72,51 +73,52 @@
     <t>COMMENTS</t>
   </si>
   <si>
-    <t>Supply of labor, testing tools and technical expertise for the Configuration of EasyGen Relay on SSR125 AVR at DG 4 &amp; DG 5.
-  Scope of works include but not limited to the following:
-  1. Wiring of Signal from EasyGen to AVR
-  2. Configuration of EasyGen relay for excitation of On-Load and Off-Load step response.
-  3. Simulation and Functional Test.</t>
+    <t>Sample scope of work 1</t>
+  </si>
+  <si>
+    <t>lot/s</t>
+  </si>
+  <si>
+    <t>sadasd</t>
+  </si>
+  <si>
+    <t>PHP</t>
+  </si>
+  <si>
+    <t>asdfasdfadsfa</t>
+  </si>
+  <si>
+    <t>fxzcasd221</t>
+  </si>
+  <si>
+    <t>Sample scope of work 2</t>
   </si>
   <si>
     <t>pc/s</t>
   </si>
   <si>
-    <t>testing</t>
-  </si>
-  <si>
-    <t>PHP</t>
-  </si>
-  <si>
-    <t>dasd</t>
-  </si>
-  <si>
-    <t>asddfgfg</t>
-  </si>
-  <si>
-    <t>testing1</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>testing2</t>
-  </si>
-  <si>
-    <t>Supply of labor, testing tools and technical expertise for the Configuration of EasyGen Relay on SSR125 AVR at DG 4 &amp; DG 51.
-  Scope of works include but not limited to the following1:
-  1. Wiring of Signal from EasyGen to AVR1
-  2. Configuration of EasyGen relay for excitation of On-Load and Off-Load step response1.
-  3. Simulation and Functional Test1.</t>
-  </si>
-  <si>
-    <t>asdsad</t>
-  </si>
-  <si>
-    <t>testing3</t>
-  </si>
-  <si>
-    <t>testing4</t>
+    <t>adsfsadf</t>
+  </si>
+  <si>
+    <t>dsafadsfd</t>
+  </si>
+  <si>
+    <t>vbgffdg</t>
+  </si>
+  <si>
+    <t>Sample scope of work 3</t>
+  </si>
+  <si>
+    <t>bot/s</t>
+  </si>
+  <si>
+    <t>sdfsadf</t>
+  </si>
+  <si>
+    <t>sadfdsf</t>
+  </si>
+  <si>
+    <t>dfgdfv xccs</t>
   </si>
   <si>
     <t>a. Price Validity</t>
@@ -125,7 +127,7 @@
     <t>b. Payment Terms</t>
   </si>
   <si>
-    <t>c. Date of Delivery</t>
+    <t>c. Work Duration</t>
   </si>
   <si>
     <t>d. Items Warranty</t>
@@ -152,10 +154,13 @@
     <t>Jonah Benares</t>
   </si>
   <si>
-    <t>Trial only11</t>
-  </si>
-  <si>
-    <t>Testing stephine11</t>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Trial only</t>
+  </si>
+  <si>
+    <t>Testing stephine</t>
   </si>
 </sst>
 </file>
@@ -192,7 +197,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,6 +210,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFf4e542"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -234,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -250,26 +261,29 @@
     <xf xfId="0" fontId="0" numFmtId="4" fillId="2" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="0" numFmtId="4" fillId="3" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -591,7 +605,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:S25"/>
+  <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A8" sqref="A8"/>
@@ -619,51 +633,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="E1" s="13"/>
+      <c r="E1" s="14"/>
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="J1" s="13"/>
-      <c r="O1" s="13"/>
+      <c r="J1" s="14"/>
+      <c r="O1" s="14"/>
     </row>
     <row r="2" spans="1:19">
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="O2" s="13"/>
+      <c r="E2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="O2" s="14"/>
     </row>
     <row r="3" spans="1:19">
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="O3" s="13"/>
+      <c r="E3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="O3" s="14"/>
     </row>
     <row r="4" spans="1:19">
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="O4" s="13"/>
+      <c r="E4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="O4" s="14"/>
     </row>
     <row r="5" spans="1:19">
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="O5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="O5" s="14"/>
     </row>
     <row r="6" spans="1:19">
-      <c r="E6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="O6" s="13"/>
+      <c r="E6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="O6" s="14"/>
     </row>
     <row r="7" spans="1:19" customHeight="1" ht="50">
       <c r="E7" s="8" t="s">
@@ -755,12 +769,12 @@
         <v>17</v>
       </c>
       <c r="C9" s="10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="16" t="s">
         <v>19</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -770,403 +784,369 @@
         <v>100</v>
       </c>
       <c r="H9" s="5">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="I9" s="2"/>
-      <c r="J9" s="15" t="s">
+      <c r="J9" s="16" t="s">
         <v>21</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="5">
-        <v>500</v>
-      </c>
-      <c r="M9" s="5">
-        <v>500</v>
+      <c r="L9" s="6">
+        <v>400</v>
+      </c>
+      <c r="M9" s="6">
+        <v>2000</v>
       </c>
       <c r="N9" s="2"/>
-      <c r="O9" s="15" t="s">
+      <c r="O9" s="16" t="s">
         <v>22</v>
       </c>
       <c r="P9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Q9" s="5">
-        <v>200</v>
-      </c>
-      <c r="R9" s="5">
-        <v>200</v>
+      <c r="Q9" s="6">
+        <v>700</v>
+      </c>
+      <c r="R9" s="6">
+        <v>3500</v>
       </c>
       <c r="S9" s="2"/>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="2"/>
       <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="9"/>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="9"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="O11" s="14"/>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="2">
+        <v>2</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="C12" s="10">
+        <v>2</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G12" s="4">
         <v>200</v>
       </c>
-      <c r="H10" s="5">
-        <v>200</v>
-      </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="K10" s="3" t="s">
+      <c r="H12" s="5">
+        <v>400</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="5">
-        <v>600</v>
-      </c>
-      <c r="M10" s="5">
-        <v>600</v>
-      </c>
-      <c r="N10" s="2"/>
-      <c r="O10" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="P10" s="3" t="s">
+      <c r="L12" s="6">
+        <v>500</v>
+      </c>
+      <c r="M12" s="6">
+        <v>1000</v>
+      </c>
+      <c r="N12" s="2"/>
+      <c r="O12" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="P12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Q10" s="5">
-        <v>300</v>
-      </c>
-      <c r="R10" s="5">
-        <v>300</v>
-      </c>
-      <c r="S10" s="2"/>
-    </row>
-    <row r="11" spans="1:19">
-      <c r="A11" s="2"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="5">
-        <v>300</v>
-      </c>
-      <c r="H11" s="5">
-        <v>300</v>
-      </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="2"/>
-    </row>
-    <row r="12" spans="1:19">
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="O12" s="13"/>
+      <c r="Q12" s="6">
+        <v>800</v>
+      </c>
+      <c r="R12" s="6">
+        <v>1600</v>
+      </c>
+      <c r="S12" s="2"/>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="2">
-        <v>2</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="10">
-        <v>2</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="4">
-        <v>400</v>
-      </c>
-      <c r="H13" s="5">
-        <v>800</v>
-      </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L13" s="5">
-        <v>700</v>
-      </c>
-      <c r="M13" s="5">
-        <v>1400</v>
-      </c>
-      <c r="N13" s="2"/>
-      <c r="O13" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="P13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q13" s="5">
-        <v>500</v>
-      </c>
-      <c r="R13" s="5">
-        <v>1000</v>
-      </c>
-      <c r="S13" s="2"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="O13" s="14"/>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="2"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="15" t="s">
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="O14" s="14"/>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="2">
+        <v>3</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="5">
-        <v>500</v>
-      </c>
-      <c r="H14" s="5">
-        <v>1000</v>
-      </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L14" s="5">
-        <v>800</v>
-      </c>
-      <c r="M14" s="5">
-        <v>1600</v>
-      </c>
-      <c r="N14" s="2"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="2"/>
-    </row>
-    <row r="15" spans="1:19">
-      <c r="A15" s="2"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="15" t="s">
+      <c r="C15" s="10">
+        <v>6</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>29</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="4">
+        <v>300</v>
+      </c>
+      <c r="H15" s="5">
+        <v>1800</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15" s="6">
         <v>600</v>
       </c>
-      <c r="H15" s="5">
-        <v>1200</v>
-      </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
+      <c r="M15" s="6">
+        <v>3600</v>
+      </c>
       <c r="N15" s="2"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
+      <c r="O15" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q15" s="6">
+        <v>900</v>
+      </c>
+      <c r="R15" s="6">
+        <v>5400</v>
+      </c>
       <c r="S15" s="2"/>
     </row>
     <row r="16" spans="1:19">
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="O16" s="13"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="O16" s="14"/>
     </row>
     <row r="17" spans="1:19">
-      <c r="B17" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="O17" s="14"/>
     </row>
     <row r="18" spans="1:19">
-      <c r="B18" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11"/>
-      <c r="R18" s="11"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="O18" s="14"/>
     </row>
     <row r="19" spans="1:19">
-      <c r="B19" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="16"/>
+      <c r="B19" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="17"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
-      <c r="J19" s="16"/>
+      <c r="J19" s="17"/>
       <c r="K19" s="11"/>
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
-      <c r="O19" s="16"/>
+      <c r="O19" s="17"/>
       <c r="P19" s="11"/>
       <c r="Q19" s="11"/>
       <c r="R19" s="11"/>
     </row>
     <row r="20" spans="1:19">
-      <c r="B20" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="16"/>
+      <c r="B20" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="17"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
-      <c r="J20" s="16"/>
+      <c r="J20" s="17"/>
       <c r="K20" s="11"/>
       <c r="L20" s="11"/>
       <c r="M20" s="11"/>
-      <c r="O20" s="16"/>
+      <c r="O20" s="17"/>
       <c r="P20" s="11"/>
       <c r="Q20" s="11"/>
       <c r="R20" s="11"/>
     </row>
     <row r="21" spans="1:19">
-      <c r="B21" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="16"/>
+      <c r="B21" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="17"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
-      <c r="J21" s="16"/>
+      <c r="J21" s="17"/>
       <c r="K21" s="11"/>
       <c r="L21" s="11"/>
       <c r="M21" s="11"/>
-      <c r="O21" s="16"/>
+      <c r="O21" s="17"/>
       <c r="P21" s="11"/>
       <c r="Q21" s="11"/>
       <c r="R21" s="11"/>
     </row>
     <row r="22" spans="1:19">
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="O22" s="13"/>
+      <c r="B22" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
     </row>
     <row r="23" spans="1:19">
-      <c r="B23" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13" t="s">
-        <v>36</v>
-      </c>
+      <c r="B23" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
       <c r="E23" s="17"/>
-      <c r="G23" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H23"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L23"/>
-      <c r="M23"/>
-      <c r="O23" s="13" t="s">
-        <v>39</v>
-      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
     </row>
     <row r="24" spans="1:19">
       <c r="B24" s="14"/>
-      <c r="C24" s="13"/>
+      <c r="C24" s="14"/>
       <c r="D24" s="14"/>
-      <c r="E24" s="18"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
+      <c r="E24" s="14"/>
+      <c r="J24" s="14"/>
       <c r="O24" s="14"/>
     </row>
     <row r="25" spans="1:19">
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="18"/>
+      <c r="G25" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13">
-        <v>33</v>
-      </c>
-      <c r="E25" s="17"/>
-      <c r="G25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="6" t="s">
+      <c r="H25"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="O25" s="13" t="s">
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="O25" s="14" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="B26" s="15"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="19"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="O26" s="15"/>
+    </row>
+    <row r="27" spans="1:19">
+      <c r="B27" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="18"/>
+      <c r="G27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="O27" s="14" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1176,12 +1156,12 @@
     <mergeCell ref="E7:I7"/>
     <mergeCell ref="J7:N7"/>
     <mergeCell ref="O7:S7"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
     <mergeCell ref="D25:E25"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="K26:M26"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>